<commit_message>
Make a new Production Template for a better Infrastructure
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49A4A47-BA33-4F16-A1A9-65A8231C4285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13535AFB-7A28-428D-8DFA-80E81AB0E821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
+    <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Kanban Boad" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -596,148 +596,148 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>COUNTA(A13:A1048576)</f>
+        <f>COUNTA(A10:A1048576)</f>
         <v>10</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>

</xml_diff>

<commit_message>
Finished developing the sign-up system
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13535AFB-7A28-428D-8DFA-80E81AB0E821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13625710-0873-489C-B07F-6D7B741447AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98147EC1-5A34-4A7A-832B-C7457EFB2E4F}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +580,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3)</f>
-        <v>0.16666666666666666</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -596,32 +596,30 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>COUNTA(A10:A1048576)</f>
+        <f>COUNTA(A5:A1048576)</f>
         <v>10</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -630,99 +628,101 @@
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Added Login and Logout system
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13625710-0873-489C-B07F-6D7B741447AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89515417-2E5E-4D79-AB43-7C9D031A57C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Not Started</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Login System</t>
-  </si>
-  <si>
-    <t>Account System: Edit Profile</t>
   </si>
   <si>
     <t>Account System: Change Password</t>
@@ -565,7 +562,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +577,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3)</f>
-        <v>0.44444444444444442</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -596,8 +593,8 @@
     </row>
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>COUNTA(A5:A1048576)</f>
-        <v>10</v>
+        <f>COUNTA(A4:A1048576)</f>
+        <v>9</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
@@ -605,12 +602,12 @@
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -619,7 +616,7 @@
     </row>
     <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -628,16 +625,16 @@
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -646,7 +643,7 @@
     </row>
     <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -655,7 +652,7 @@
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -664,7 +661,7 @@
     </row>
     <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -673,7 +670,7 @@
     </row>
     <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -682,22 +679,20 @@
     </row>
     <row r="12" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>

</xml_diff>

<commit_message>
Developed Password Recovery System
A 3-part system that asks for your email to reset password on, then verifying your identity through verification codes, and finally changing and confirming your password
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89515417-2E5E-4D79-AB43-7C9D031A57C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C64370D-B630-47AE-A933-787B8D0CF2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -562,7 +562,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +577,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3)</f>
-        <v>0.5</v>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -594,7 +594,7 @@
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>COUNTA(A4:A1048576)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
@@ -602,12 +602,12 @@
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -616,7 +616,7 @@
     </row>
     <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -625,7 +625,7 @@
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -634,7 +634,7 @@
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -643,7 +643,7 @@
     </row>
     <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -652,7 +652,7 @@
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -661,7 +661,7 @@
     </row>
     <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -670,7 +670,7 @@
     </row>
     <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -678,9 +678,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>12</v>
@@ -689,7 +687,9 @@
     <row r="13" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>

</xml_diff>

<commit_message>
Added verify token route
Ensures that authorized routes aren't visited by users who do not have valid tokens
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C64370D-B630-47AE-A933-787B8D0CF2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E769E973-9182-46DD-9EA7-805D515E3127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -562,7 +562,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +576,7 @@
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="3">
-        <f>C3 / (C3 + A3)</f>
+        <f>C3 / (C3 + A3 + B3)</f>
         <v>0.55555555555555558</v>
       </c>
     </row>
@@ -594,11 +594,11 @@
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>COUNTA(A4:A1048576)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
@@ -609,7 +609,9 @@
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -652,7 +654,7 @@
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -661,7 +663,7 @@
     </row>
     <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -669,9 +671,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Developed Change Email System
Allow users to change their email during login
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E769E973-9182-46DD-9EA7-805D515E3127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04EBCE4-354F-4C97-BD11-3D4DD2C928C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t>Update Books System</t>
   </si>
   <si>
-    <t>User Idle System</t>
-  </si>
-  <si>
     <t>Website UI</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Create cloud infrastructure</t>
+  </si>
+  <si>
+    <t>Account System: Activity Log</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +577,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3 + B3)</f>
-        <v>0.55555555555555558</v>
+        <v>0.61111111111111116</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -598,20 +598,18 @@
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -627,16 +625,16 @@
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -645,7 +643,7 @@
     </row>
     <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -663,7 +661,7 @@
     </row>
     <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -694,7 +692,9 @@
     <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>

</xml_diff>

<commit_message>
Implemented password change system during login activity
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04EBCE4-354F-4C97-BD11-3D4DD2C928C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1189D278-2441-45CA-900D-EB4589EAB9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -577,7 +577,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3 + B3)</f>
-        <v>0.61111111111111116</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -594,7 +594,7 @@
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>COUNTA(A4:A1048576)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
@@ -602,7 +602,7 @@
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
     </row>
     <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -625,7 +625,7 @@
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -634,7 +634,7 @@
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -643,7 +643,7 @@
     </row>
     <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -652,7 +652,7 @@
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
@@ -660,9 +660,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -699,7 +697,9 @@
     <row r="15" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>

</xml_diff>

<commit_message>
Implemented Pagination for each user's activity logs
Allows users to go through pages of activity logs instead of retrieving all of them in one go
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1189D278-2441-45CA-900D-EB4589EAB9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15284A2F-BD70-48B6-B78F-0196C7D50848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -562,7 +562,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +577,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3 + B3)</f>
-        <v>0.66666666666666663</v>
+        <v>0.72222222222222221</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -594,7 +594,7 @@
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>COUNTA(A4:A1048576)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
@@ -602,7 +602,7 @@
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
@@ -651,9 +651,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -704,7 +702,9 @@
     <row r="16" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>

</xml_diff>

<commit_message>
Initialized Add Book and Retrieve all Books API
Allows users to add a book. Also allows them to retrieve all books. Will be edited later to add pagination
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15284A2F-BD70-48B6-B78F-0196C7D50848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B4A8CE-A4D8-485D-8949-4043849A6F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Not Started</t>
   </si>
@@ -89,19 +89,22 @@
     <t>Add Books System</t>
   </si>
   <si>
-    <t>Update Books System</t>
-  </si>
-  <si>
     <t>Website UI</t>
   </si>
   <si>
-    <t>View Book Instance Page</t>
-  </si>
-  <si>
     <t>Create cloud infrastructure</t>
   </si>
   <si>
     <t>Account System: Activity Log</t>
+  </si>
+  <si>
+    <t>Edit a Book System</t>
+  </si>
+  <si>
+    <t>View a Book Instance Page</t>
+  </si>
+  <si>
+    <t>View all Books System</t>
   </si>
 </sst>
 </file>
@@ -562,7 +565,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +580,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3 + B3)</f>
-        <v>0.72222222222222221</v>
+        <v>0.68421052631578949</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -594,11 +597,11 @@
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>COUNTA(A4:A1048576)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
@@ -609,16 +612,20 @@
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
@@ -629,12 +636,12 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -642,9 +649,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>9</v>
@@ -703,7 +708,7 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Initiated a View book instance page
Also finished the main functionalities of adding a book. View book instance page still needs an add, update, and delete note apis
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B4A8CE-A4D8-485D-8949-4043849A6F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198F184E-B253-43E2-AFE7-A8FD4724C527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Not Started</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Account System: Change Email</t>
   </si>
   <si>
-    <t>Homepage System</t>
-  </si>
-  <si>
     <t>Add Books System</t>
   </si>
   <si>
@@ -105,6 +102,12 @@
   </si>
   <si>
     <t>View all Books System</t>
+  </si>
+  <si>
+    <t>Dashboard System</t>
+  </si>
+  <si>
+    <t>Search Book System</t>
   </si>
 </sst>
 </file>
@@ -565,7 +568,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +583,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3 + B3)</f>
-        <v>0.68421052631578949</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -605,15 +608,15 @@
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
@@ -621,10 +624,10 @@
     </row>
     <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>8</v>
@@ -632,16 +635,16 @@
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -708,13 +711,15 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>

</xml_diff>

<commit_message>
Finished developing REST API for books and notes
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198F184E-B253-43E2-AFE7-A8FD4724C527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420BD629-228A-425E-9A8A-0B66A86ED242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -565,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98147EC1-5A34-4A7A-832B-C7457EFB2E4F}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +583,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3 + B3)</f>
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -600,15 +600,15 @@
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>COUNTA(A4:A1048576)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
@@ -624,18 +624,16 @@
     </row>
     <row r="5" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -643,9 +641,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -724,12 +720,16 @@
     <row r="18" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
@@ -745,6 +745,16 @@
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added pagination for Books View.
Also added a search button for books view. Results are limited to 5 books only
</commit_message>
<xml_diff>
--- a/documents/Kanban Board.xlsx
+++ b/documents/Kanban Board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Downloads\NoteStrip\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420BD629-228A-425E-9A8A-0B66A86ED242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2DB278-7E89-4CBE-BDAF-EAF83D60C6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2805" windowWidth="16695" windowHeight="11700" xr2:uid="{49F89782-41B1-45E3-9437-FA87AC367B9B}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +583,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="3">
         <f>C3 / (C3 + A3 + B3)</f>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
@@ -600,24 +600,22 @@
     <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>COUNTA(A4:A1048576)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <f>COUNTA(B4:B1048576)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <f>COUNTA(C4:C1048576)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -632,9 +630,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>17</v>
@@ -734,12 +730,16 @@
     <row r="20" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>

</xml_diff>